<commit_message>
Tweaks to Forensic Science data files.
Also giving the final_analysis.R copy a more realistic name.
</commit_message>
<xml_diff>
--- a/files/file-org/forensic-science/data1.xlsx
+++ b/files/file-org/forensic-science/data1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="0" windowWidth="25280" windowHeight="15320" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="gapminderDataFiveYear.tsv" sheetId="1" r:id="rId1"/>
+    <sheet name="gapminder subset" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -870,7 +870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1693"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>

</xml_diff>